<commit_message>
I created a working model for adding a record to a table from a telegram
</commit_message>
<xml_diff>
--- a/kogda_igra_telegram_bot/sample.xlsx
+++ b/kogda_igra_telegram_bot/sample.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView windowProtection="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
@@ -586,35 +586,92 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>13 июля 2021</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>15 июля 2021</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>БзР</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>Джон Сильвер</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>захват точек</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>@silver</t>
         </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>дата</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>дата конец</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Название</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Организатор</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>педулово</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1205233811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor corrections have been made
</commit_message>
<xml_diff>
--- a/kogda_igra_telegram_bot/sample.xlsx
+++ b/kogda_igra_telegram_bot/sample.xlsx
@@ -453,20 +453,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView windowProtection="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8"/>
   <cols>
-    <col width="16.530612244898" customWidth="1" style="2" min="1" max="2"/>
-    <col width="23.1530612244898" customWidth="1" style="2" min="3" max="3"/>
-    <col width="14.9744897959184" customWidth="1" style="2" min="4" max="4"/>
-    <col width="9.05102040816327" customWidth="1" style="2" min="5" max="5"/>
-    <col width="12.1581632653061" customWidth="1" style="2" min="6" max="6"/>
-    <col width="8.36734693877551" customWidth="1" style="2" min="7" max="1025"/>
+    <col width="16.3316326530612" customWidth="1" style="2" min="1" max="2"/>
+    <col width="22.8112244897959" customWidth="1" style="2" min="3" max="3"/>
+    <col width="14.7142857142857" customWidth="1" style="2" min="4" max="4"/>
+    <col width="8.77551020408163" customWidth="1" style="2" min="5" max="5"/>
+    <col width="11.8775510204082" customWidth="1" style="2" min="6" max="6"/>
+    <col width="8.23469387755102" customWidth="1" style="2" min="7" max="1025"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.8" customHeight="1" s="3">
@@ -553,7 +553,7 @@
         </is>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15" customHeight="1" s="3">
       <c r="A4" s="2" t="inlineStr">
         <is>
           <t>25 сентября 2021</t>
@@ -585,7 +585,7 @@
         </is>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15" customHeight="1" s="3">
       <c r="A5" s="2" t="inlineStr">
         <is>
           <t>13 июля 2021</t>
@@ -617,61 +617,252 @@
         </is>
       </c>
     </row>
-    <row r="7">
+    <row r="6" ht="15" customHeight="1" s="3">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="3">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>дата</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>дата конец</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Название</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Организатор</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>дата</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>дата конец</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Название</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Организатор</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
           <t>педулово</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="F7" s="2" t="n">
         <v>1205233811</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="3">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>21 января</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>23 февраля</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>БЗР</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Вадимир</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>захват точек</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>1205233811</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" s="3">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>12 сентября</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>13 сентября</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>СТАЛКЕР</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Тур</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>Ролевая</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>d1m0nnch1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>12 сентября 2222</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>15 октября 2222</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>мероприятие</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Дроид групп</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>Удержание</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>d1m0nnch1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>1 января 2023</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>3 января 2023</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Битва за Мандарины</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Вадимир</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>Охота за конфетами</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>d1m0nnch1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>1 февраля 2023</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>4 февраля 2023</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>Февральский мороз</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>ПП</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>встречный бой</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>d1m0nnch1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>13 марта 2022</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>15 марта 2022</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>название</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>организатор</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>игра</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>d1m0nnch1k</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added buttons to the message
</commit_message>
<xml_diff>
--- a/kogda_igra_telegram_bot/sample.xlsx
+++ b/kogda_igra_telegram_bot/sample.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -933,17 +933,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>тест11</t>
+          <t>тест 11</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>тест11</t>
+          <t>тест 11</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>тест11</t>
+          <t>тест 11</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -973,17 +973,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Шарометный бой</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Дарт Вейдер</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Уничтожение повстанцев</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -1013,17 +1013,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Шарометный бой</t>
+          <t>тест11</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Дарт Вейдер</t>
+          <t>тест11</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Уничтожение повстанцев</t>
+          <t>тест11</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -1198,32 +1198,32 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>15.09.2021</t>
+          <t>06.09.2021</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2021-09-15</t>
+          <t>2021-09-06</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>19.09.2021</t>
+          <t>10.09.2021</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Битва за ресурсы</t>
+          <t>Мероприятие игры в страйкбол</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Вадимир</t>
+          <t>Самый лучший</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Захват точек</t>
+          <t>клюквомет</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1232,38 +1232,38 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16.09.2021</t>
+          <t>15.09.2021</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2021-09-16</t>
+          <t>2021-09-15</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>21.09.2021</t>
+          <t>19.09.2021</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ИСАФ</t>
+          <t>Битва за ресурсы</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>HQ</t>
+          <t>Вадимир</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>милсим</t>
+          <t>Захват точек</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1272,38 +1272,38 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>01.10.2021</t>
+          <t>16.09.2021</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-09-16</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>03.10.2021</t>
+          <t>21.09.2021</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Алкосталкер</t>
+          <t>ИСАФ</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Алкоорганизатор</t>
+          <t>HQ</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Ролевое бухалово</t>
+          <t>милсим</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1312,46 +1312,126 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>17.09.2021</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2021-09-17</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>18.09.2021</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Самая лучшая игра</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Самый лучший организатор</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Самый лучший тип игр</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>d1m0nnch1k</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>01.10.2021</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2021-10-01</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>03.10.2021</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Алкосталкер</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Алкоорганизатор</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Ролевое бухалово</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>d1m0nnch1k</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>15.10.2021</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>2021-10-15</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>18.10.2021</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>йцуке</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>фывап</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>ячсми</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>d1m0nnch1k</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
function of the edit buttons was made (change the name, type, delete event)
</commit_message>
<xml_diff>
--- a/kogda_igra_telegram_bot/sample.xlsx
+++ b/kogda_igra_telegram_bot/sample.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -773,17 +773,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>Тест правки названия</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>тест8</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>тест8</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>тест8</t>
+          <t>Измененный тип игры</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -933,17 +933,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Шарометный бой</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Дарт Вейдер</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Уничтожение повстанцев</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -973,17 +973,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Шарометный бой</t>
+          <t>тест 11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Дарт Вейдер</t>
+          <t>тест 11</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Уничтожение повстанцев</t>
+          <t>тест 11</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -992,38 +992,38 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>23.08.2021</t>
+          <t>29.08.2021</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2021-08-23</t>
+          <t>2021-08-29</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>25.08.2021</t>
+          <t>30.08.2021</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>тест11</t>
+          <t>Бухач</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>тест11</t>
+          <t>Джон и Джон</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>тест11</t>
+          <t>Фестиваль</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1032,38 +1032,38 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>29.08.2021</t>
+          <t>01.09.2021</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2021-08-29</t>
+          <t>2021-09-01</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>30.08.2021</t>
+          <t>03.09.2021</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Бухач</t>
+          <t>тест 13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Джон и Джон</t>
+          <t>тест 13</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Фестиваль</t>
+          <t>тест 13</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1072,38 +1072,38 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>01.09.2021</t>
+          <t>03.09.2021</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2021-09-01</t>
+          <t>2021-09-03</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>03.09.2021</t>
+          <t>05.09.2021</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>тест 13</t>
+          <t>фыв</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>тест 13</t>
+          <t>фывфывфыв</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>тест 13</t>
+          <t>фывфывфыв</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1112,38 +1112,38 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03.09.2021</t>
+          <t>06.09.2021</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2021-09-03</t>
+          <t>2021-09-06</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>05.09.2021</t>
+          <t>09.09.2021</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>фыв</t>
+          <t>Трудно быть зомби</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>фывфывфыв</t>
+          <t>ФВСТИ</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>фывфывфыв</t>
+          <t>Выживание</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
@@ -1168,22 +1168,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>09.09.2021</t>
+          <t>10.09.2021</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Трудно быть зомби</t>
+          <t>Мероприятие игры в страйкбол</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>ФВСТИ</t>
+          <t>Самый лучший</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Выживание</t>
+          <t>клюквомет</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1192,38 +1192,38 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06.09.2021</t>
+          <t>15.09.2021</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2021-09-06</t>
+          <t>2021-09-15</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>10.09.2021</t>
+          <t>19.09.2021</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Мероприятие игры в страйкбол</t>
+          <t>Битва за ресурсы</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Самый лучший</t>
+          <t>Вадимир</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>клюквомет</t>
+          <t>Захват точек</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1232,38 +1232,38 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>15.09.2021</t>
+          <t>16.09.2021</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2021-09-15</t>
+          <t>2021-09-16</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>19.09.2021</t>
+          <t>21.09.2021</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Битва за ресурсы</t>
+          <t>ИСАФ</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Вадимир</t>
+          <t>HQ</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Захват точек</t>
+          <t>милсим</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1272,38 +1272,38 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>16.09.2021</t>
+          <t>17.09.2021</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2021-09-16</t>
+          <t>2021-09-17</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>21.09.2021</t>
+          <t>18.09.2021</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ИСАФ</t>
+          <t>Самая лучшая игра</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>HQ</t>
+          <t>Самый лучший организатор</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>милсим</t>
+          <t>Самый лучший тип игр</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1312,38 +1312,38 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17.09.2021</t>
+          <t>01.10.2021</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2021-09-17</t>
+          <t>2021-10-01</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>18.09.2021</t>
+          <t>03.10.2021</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Самая лучшая игра</t>
+          <t>Алкосталкер</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Самый лучший организатор</t>
+          <t>Алкоорганизатор</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Самый лучший тип игр</t>
+          <t>Ролевое бухалово</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1352,38 +1352,38 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>01.10.2021</t>
+          <t>15.10.2021</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-15</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>03.10.2021</t>
+          <t>18.10.2021</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Алкосталкер</t>
+          <t>Вменяемое название</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Алкоорганизатор</t>
+          <t>фывап</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Ролевое бухалово</t>
+          <t>ячсми</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1392,46 +1392,6 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>15.10.2021</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>2021-10-15</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>18.10.2021</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>йцуке</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>фывап</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>ячсми</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H25" t="n">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The function of changing the dates of the event is finished, the work on the comments to the code is started
</commit_message>
<xml_diff>
--- a/kogda_igra_telegram_bot/sample.xlsx
+++ b/kogda_igra_telegram_bot/sample.xlsx
@@ -718,12 +718,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>10.08.2021</t>
+          <t>11.08.2021</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2021-08-10</t>
+          <t>2021-08-11</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -933,17 +933,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Шарометный бой</t>
+          <t>тест 11</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Дарт Вейдер</t>
+          <t>тест 11</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Уничтожение повстанцев</t>
+          <t>тест 11</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -973,17 +973,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Шарометный бой</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Дарт Вейдер</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Уничтожение повстанцев</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>фыв</t>
+          <t>Игра в домино</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1198,17 +1198,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>15.09.2021</t>
+          <t>16.09.2021</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2021-09-15</t>
+          <t>2021-09-16</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>19.09.2021</t>
+          <t>20.09.2021</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1238,32 +1238,32 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16.09.2021</t>
+          <t>17.09.2021</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2021-09-16</t>
+          <t>2021-09-17</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>21.09.2021</t>
+          <t>18.09.2021</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ИСАФ</t>
+          <t>Самая лучшая игра</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>HQ</t>
+          <t>Самый лучший организатор</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>милсим</t>
+          <t>Самый лучший тип игр</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1272,38 +1272,38 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>17.09.2021</t>
+          <t>20.09.2021</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2021-09-17</t>
+          <t>2021-09-20</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>18.09.2021</t>
+          <t>23.09.2021</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Самая лучшая игра</t>
+          <t>ИСАФ</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Самый лучший организатор</t>
+          <t>HQ</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Самый лучший тип игр</t>
+          <t>милсим</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">

</xml_diff>

<commit_message>
Added description and corrected error when re-adding an ad
</commit_message>
<xml_diff>
--- a/kogda_igra_telegram_bot/sample.xlsx
+++ b/kogda_igra_telegram_bot/sample.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,41 +478,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15.07.2021</t>
+          <t>01.01.2020</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2021-07-15</t>
+          <t>2020-01-01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>18.07.2021</t>
+          <t>01.01.2030</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>тест7</t>
+          <t>хуй</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>тест7</t>
+          <t>хуй-хнает-кто</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>тест7</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
+          <t>карманный биллиард</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -528,7 +524,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15.07.2021</t>
+          <t>18.07.2021</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -552,38 +548,38 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16.07.2021</t>
+          <t>15.07.2021</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2021-07-16</t>
+          <t>2021-07-15</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>21.07.2021</t>
+          <t>15.07.2021</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Название мероприятия</t>
+          <t>тест7</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Организатор мероприятия</t>
+          <t>тест7</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Тип игры</t>
+          <t>тест7</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -592,38 +588,38 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>28.07.2021</t>
+          <t>16.07.2021</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2021-07-28</t>
+          <t>2021-07-16</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>03.09.2021</t>
+          <t>21.07.2021</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Тестовое мероприятие по игре в страйкбол</t>
+          <t>Название мероприятия</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Оргруппа орги</t>
+          <t>Организатор мероприятия</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Битва за бутылку</t>
+          <t>Тип игры</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -632,38 +628,38 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>30.07.2021</t>
+          <t>28.07.2021</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2021-07-30</t>
+          <t>2021-07-28</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>09.08.2021</t>
+          <t>03.09.2021</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Битва за ресурсы2</t>
+          <t>Тестовое мероприятие по игре в страйкбол</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Вадимир</t>
+          <t>Оргруппа орги</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Захват точек</t>
+          <t>Битва за бутылку</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -672,38 +668,38 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01.08.2021</t>
+          <t>30.07.2021</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2021-08-01</t>
+          <t>2021-07-30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>03.08.2021</t>
+          <t>09.08.2021</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>тест10</t>
+          <t>Битва за ресурсы2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>тест10</t>
+          <t>Вадимир</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>тест10</t>
+          <t>Захват точек</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -712,38 +708,38 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>11.08.2021</t>
+          <t>01.08.2021</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2021-08-11</t>
+          <t>2021-08-01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>12.08.2021</t>
+          <t>03.08.2021</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Мероприятие мероприятий</t>
+          <t>тест10</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Организаторский Организатор</t>
+          <t>тест10</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>игрушечка</t>
+          <t>тест10</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -752,38 +748,38 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>15.08.2021</t>
+          <t>09.08.2021</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2021-08-15</t>
+          <t>2021-08-09</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>18.08.2021</t>
+          <t>09.08.2021</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Тест правки названия</t>
+          <t>11111</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>тест8</t>
+          <t>22222</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Измененный тип игры</t>
+          <t>33333</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -792,38 +788,38 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16.08.2021</t>
+          <t>09.08.2021</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2021-08-16</t>
+          <t>2021-08-09</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>18.08.2021</t>
+          <t>10.08.2021</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>тест9</t>
+          <t>название</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>тест9</t>
+          <t>123</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>тест9</t>
+          <t>педулово</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -832,118 +828,118 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18.08.2021</t>
+          <t>10.08.2021</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2021-08-18</t>
+          <t>2021-08-10</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>20.08.2021</t>
+          <t>11.08.2021</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>тест 12</t>
+          <t>мероприятие 1</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>тест 12</t>
+          <t>я</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>тест 12</t>
+          <t>игра</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>d1m0nnch1k</t>
+          <t>elvirarah</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18.08.2021</t>
+          <t>12.08.2021</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2021-08-18</t>
+          <t>2021-08-12</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>20.08.2021</t>
+          <t>13.08.2021</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>ИГРА ПОД НАЗВАНИЕМ "ИГРА"</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Организатор #неТорт</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>Флешбеки из Вьетнама имени Джонни</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>d1m0nnch1k</t>
+          <t>dm_ruslanowi4</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>23.08.2021</t>
+          <t>20.09.2021</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2021-08-23</t>
+          <t>2021-09-20</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>25.08.2021</t>
+          <t>23.09.2021</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>ИСАФ</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>HQ</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>тест 11</t>
+          <t>милсим</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -952,78 +948,74 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>23.08.2021</t>
+          <t>29.09.2021</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2021-08-23</t>
+          <t>2021-09-29</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>25.08.2021</t>
+          <t>03.10.2021</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Шарометный бой</t>
+          <t>Осколки Миров</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Дарт Вейдер</t>
+          <t>Олег Черный https://m.vk.com/worldsshards</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Уничтожение повстанцев</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
+          <t>Фентези ПРИ</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>29.08.2021</t>
+          <t>01.10.2021</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2021-08-29</t>
+          <t>2021-10-01</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>30.08.2021</t>
+          <t>03.10.2021</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Бухач</t>
+          <t>Алкосталкер</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Джон и Джон</t>
+          <t>Алкоорганизатор</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Фестиваль</t>
+          <t>Ролевое бухалово</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1032,38 +1024,38 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>01.09.2021</t>
+          <t>10.10.2021</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2021-09-01</t>
+          <t>2021-10-10</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>03.09.2021</t>
+          <t>11.10.2021</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>тест 13</t>
+          <t>мероприятин</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>тест 13</t>
+          <t>орг</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>тест 13</t>
+          <t>игр</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1072,327 +1064,7 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>03.09.2021</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2021-09-03</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>05.09.2021</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Игра в домино</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>фывфывфыв</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>фывфывфыв</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>06.09.2021</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2021-09-06</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>09.09.2021</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Трудно быть зомби</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>ФВСТИ</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Выживание</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>06.09.2021</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2021-09-06</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>10.09.2021</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Мероприятие игры в страйкбол</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Самый лучший</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>клюквомет</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>16.09.2021</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2021-09-16</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>20.09.2021</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Битва за ресурсы</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Вадимир</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Захват точек</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>17.09.2021</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>2021-09-17</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>18.09.2021</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Самая лучшая игра</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Самый лучший организатор</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Самый лучший тип игр</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>20.09.2021</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>2021-09-20</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>23.09.2021</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>ИСАФ</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>HQ</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>милсим</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>01.10.2021</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2021-10-01</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>03.10.2021</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Алкосталкер</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Алкоорганизатор</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Ролевое бухалово</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>15.10.2021</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>2021-10-15</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>18.10.2021</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Вменяемое название</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>фывап</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>ячсми</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>d1m0nnch1k</t>
-        </is>
-      </c>
-      <c r="H24" t="n">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>